<commit_message>
uploading all eddy data
Still missing some information
</commit_message>
<xml_diff>
--- a/eddy/TK3_to_NetCDF.xlsx
+++ b/eddy/TK3_to_NetCDF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexd/Documents/GitHub/scripts/eddy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD39336C-7202-4673-AC43-8D0074FCD020}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29A233D-3865-484C-9BB6-DFCDC687328F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global attributes" sheetId="3" r:id="rId1"/>
@@ -966,7 +966,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1653,6 +1653,27 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1670,27 +1691,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1931,24 +1931,24 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="74.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="78.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="74.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>297</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="70" t="s">
         <v>299</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>132</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
         <v>134</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>136</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
         <v>137</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>138</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>139</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="46" t="s">
         <v>226</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="46" t="s">
         <v>204</v>
       </c>
@@ -2034,23 +2034,23 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="136" t="s">
         <v>233</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="138" t="s">
         <v>300</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="139"/>
       <c r="B4" s="85" t="s">
         <v>98</v>
@@ -2115,7 +2115,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="139"/>
       <c r="B5" s="86" t="s">
         <v>107</v>
@@ -2136,7 +2136,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1">
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="140"/>
       <c r="B6" s="133" t="s">
         <v>305</v>
@@ -2157,7 +2157,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="9" customFormat="1">
+    <row r="7" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="137" t="s">
         <v>144</v>
       </c>
@@ -2178,18 +2178,18 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="F8" s="25"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E10" s="47"/>
       <c r="G10" s="28"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E11" s="47"/>
       <c r="G11" s="28"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E12" s="47"/>
     </row>
   </sheetData>
@@ -2208,60 +2208,60 @@
   <dimension ref="A1:CN44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="AF1" activePane="topRight" state="frozen"/>
       <selection activeCell="B24" sqref="B24"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7:D7"/>
+      <selection pane="topRight" activeCell="AZ12" sqref="AZ12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="48" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="36" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="36" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="31" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="24.42578125" customWidth="1"/>
-    <col min="40" max="40" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="27.42578125" customWidth="1"/>
+    <col min="38" max="38" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="24.5" customWidth="1"/>
+    <col min="40" max="40" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="27.5" customWidth="1"/>
     <col min="44" max="44" width="30" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="32" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="60" max="63" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="64" max="92" width="11.5703125" style="1" bestFit="1"/>
+    <col min="57" max="57" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="60" max="63" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="92" width="11.5" style="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" s="33" customFormat="1">
-      <c r="A1" s="147" t="s">
+    <row r="1" spans="1:92" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="144" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="148"/>
+      <c r="B1" s="145"/>
       <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
@@ -2475,11 +2475,11 @@
       <c r="CM1" s="32"/>
       <c r="CN1" s="32"/>
     </row>
-    <row r="2" spans="1:92" s="32" customFormat="1">
-      <c r="A2" s="149" t="s">
+    <row r="2" spans="1:92" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="146" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="150"/>
+      <c r="B2" s="147"/>
       <c r="C2" s="39" t="s">
         <v>63</v>
       </c>
@@ -2664,11 +2664,11 @@
         <v>0.66210420000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:92" s="32" customFormat="1">
-      <c r="A3" s="149" t="s">
+    <row r="3" spans="1:92" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="146" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="150"/>
+      <c r="B3" s="147"/>
       <c r="C3" s="35" t="s">
         <v>67</v>
       </c>
@@ -2853,11 +2853,11 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:92" s="38" customFormat="1">
-      <c r="A4" s="149" t="s">
+    <row r="4" spans="1:92" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="146" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="150"/>
+      <c r="B4" s="147"/>
       <c r="C4" s="41" t="s">
         <v>125</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="BJ4" s="41"/>
       <c r="BK4" s="41"/>
     </row>
-    <row r="5" spans="1:92" s="38" customFormat="1">
+    <row r="5" spans="1:92" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="116"/>
       <c r="B5" s="117"/>
       <c r="C5" s="66"/>
@@ -3057,7 +3057,7 @@
       <c r="BJ5" s="66"/>
       <c r="BK5" s="66"/>
     </row>
-    <row r="6" spans="1:92" s="32" customFormat="1">
+    <row r="6" spans="1:92" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="118"/>
       <c r="B6" s="118"/>
       <c r="C6" s="42"/>
@@ -3066,16 +3066,157 @@
       <c r="F6" s="42"/>
       <c r="G6" s="42"/>
       <c r="H6" s="42"/>
-    </row>
-    <row r="7" spans="1:92" s="33" customFormat="1">
-      <c r="A7" s="147" t="s">
+      <c r="O6" s="32">
+        <v>0</v>
+      </c>
+      <c r="P6" s="32">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="32">
+        <v>2</v>
+      </c>
+      <c r="R6" s="32">
+        <v>3</v>
+      </c>
+      <c r="S6" s="32">
+        <v>4</v>
+      </c>
+      <c r="T6" s="32">
+        <v>5</v>
+      </c>
+      <c r="U6" s="32">
+        <v>6</v>
+      </c>
+      <c r="V6" s="32">
+        <v>7</v>
+      </c>
+      <c r="W6" s="32">
+        <v>8</v>
+      </c>
+      <c r="X6" s="32">
+        <v>9</v>
+      </c>
+      <c r="Y6" s="32">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="32">
+        <v>11</v>
+      </c>
+      <c r="AA6" s="32">
+        <v>12</v>
+      </c>
+      <c r="AB6" s="32">
+        <v>13</v>
+      </c>
+      <c r="AC6" s="32">
+        <v>14</v>
+      </c>
+      <c r="AD6" s="32">
+        <v>15</v>
+      </c>
+      <c r="AE6" s="32">
+        <v>16</v>
+      </c>
+      <c r="AF6" s="32">
+        <v>17</v>
+      </c>
+      <c r="AG6" s="32">
+        <v>19</v>
+      </c>
+      <c r="AH6" s="32">
+        <v>20</v>
+      </c>
+      <c r="AI6" s="32">
+        <v>21</v>
+      </c>
+      <c r="AJ6" s="32">
+        <v>22</v>
+      </c>
+      <c r="AK6" s="32">
+        <v>23</v>
+      </c>
+      <c r="AM6" s="32">
+        <v>24</v>
+      </c>
+      <c r="AN6" s="32">
+        <v>25</v>
+      </c>
+      <c r="AO6" s="32">
+        <v>26</v>
+      </c>
+      <c r="AP6" s="32">
+        <v>27</v>
+      </c>
+      <c r="AQ6" s="32">
+        <v>28</v>
+      </c>
+      <c r="AR6" s="32">
+        <v>29</v>
+      </c>
+      <c r="AS6" s="32">
+        <v>30</v>
+      </c>
+      <c r="AT6" s="32">
+        <v>31</v>
+      </c>
+      <c r="AU6" s="32">
+        <v>32</v>
+      </c>
+      <c r="AV6" s="32">
+        <v>33</v>
+      </c>
+      <c r="AW6" s="32">
+        <v>34</v>
+      </c>
+      <c r="AY6" s="32">
+        <v>35</v>
+      </c>
+      <c r="AZ6" s="32">
+        <v>36</v>
+      </c>
+      <c r="BA6" s="32">
+        <v>37</v>
+      </c>
+      <c r="BB6" s="32">
+        <v>38</v>
+      </c>
+      <c r="BC6" s="32">
+        <v>39</v>
+      </c>
+      <c r="BD6" s="32">
+        <v>40</v>
+      </c>
+      <c r="BE6" s="32">
+        <v>41</v>
+      </c>
+      <c r="BF6" s="32">
+        <v>42</v>
+      </c>
+      <c r="BG6" s="32">
+        <v>43</v>
+      </c>
+      <c r="BH6" s="32">
+        <v>44</v>
+      </c>
+      <c r="BI6" s="32">
+        <v>45</v>
+      </c>
+      <c r="BJ6" s="32">
+        <v>46</v>
+      </c>
+      <c r="BK6" s="32">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:92" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="144" t="s">
         <v>233</v>
       </c>
-      <c r="B7" s="148"/>
-      <c r="C7" s="145" t="s">
+      <c r="B7" s="145"/>
+      <c r="C7" s="152" t="s">
         <v>229</v>
       </c>
-      <c r="D7" s="146"/>
+      <c r="D7" s="153"/>
       <c r="E7" s="89" t="s">
         <v>85</v>
       </c>
@@ -3233,17 +3374,17 @@
       <c r="CM7" s="32"/>
       <c r="CN7" s="32"/>
     </row>
-    <row r="8" spans="1:92" s="32" customFormat="1" ht="14.45" customHeight="1">
-      <c r="A8" s="151" t="s">
+    <row r="8" spans="1:92" s="32" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="141" t="s">
         <v>300</v>
       </c>
       <c r="B8" s="113" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="141" t="s">
+      <c r="C8" s="148" t="s">
         <v>308</v>
       </c>
-      <c r="D8" s="142"/>
+      <c r="D8" s="149"/>
       <c r="E8" s="39" t="s">
         <v>89</v>
       </c>
@@ -3336,15 +3477,15 @@
       <c r="BJ8" s="63"/>
       <c r="BK8" s="63"/>
     </row>
-    <row r="9" spans="1:92" s="32" customFormat="1" ht="30">
-      <c r="A9" s="152"/>
+    <row r="9" spans="1:92" s="32" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="142"/>
       <c r="B9" s="113" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="141" t="s">
+      <c r="C9" s="148" t="s">
         <v>308</v>
       </c>
-      <c r="D9" s="142"/>
+      <c r="D9" s="149"/>
       <c r="E9" s="89" t="s">
         <v>248</v>
       </c>
@@ -3473,15 +3614,15 @@
       <c r="BJ9" s="53"/>
       <c r="BK9" s="53"/>
     </row>
-    <row r="10" spans="1:92" s="38" customFormat="1">
-      <c r="A10" s="152"/>
+    <row r="10" spans="1:92" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="142"/>
       <c r="B10" s="114" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="143" t="s">
+      <c r="C10" s="150" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="144"/>
+      <c r="D10" s="151"/>
       <c r="E10" s="41" t="s">
         <v>109</v>
       </c>
@@ -3610,15 +3751,15 @@
       <c r="BJ10" s="56"/>
       <c r="BK10" s="56"/>
     </row>
-    <row r="11" spans="1:92" s="98" customFormat="1">
-      <c r="A11" s="152"/>
+    <row r="11" spans="1:92" s="98" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="142"/>
       <c r="B11" s="115" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="141" t="s">
+      <c r="C11" s="148" t="s">
         <v>308</v>
       </c>
-      <c r="D11" s="142"/>
+      <c r="D11" s="149"/>
       <c r="E11" s="90" t="s">
         <v>124</v>
       </c>
@@ -3745,15 +3886,15 @@
       <c r="BJ11" s="95"/>
       <c r="BK11" s="95"/>
     </row>
-    <row r="12" spans="1:92" s="38" customFormat="1" ht="30">
-      <c r="A12" s="152"/>
+    <row r="12" spans="1:92" s="38" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="142"/>
       <c r="B12" s="115" t="s">
         <v>223</v>
       </c>
-      <c r="C12" s="141" t="s">
+      <c r="C12" s="148" t="s">
         <v>308</v>
       </c>
-      <c r="D12" s="142"/>
+      <c r="D12" s="149"/>
       <c r="E12" s="69" t="s">
         <v>260</v>
       </c>
@@ -3834,15 +3975,15 @@
       <c r="BJ12" s="56"/>
       <c r="BK12" s="56"/>
     </row>
-    <row r="13" spans="1:92" s="1" customFormat="1">
-      <c r="A13" s="152"/>
+    <row r="13" spans="1:92" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="142"/>
       <c r="B13" s="112" t="s">
         <v>230</v>
       </c>
-      <c r="C13" s="141" t="s">
+      <c r="C13" s="148" t="s">
         <v>308</v>
       </c>
-      <c r="D13" s="142"/>
+      <c r="D13" s="149"/>
       <c r="E13" s="120" t="s">
         <v>308</v>
       </c>
@@ -3907,15 +4048,15 @@
       <c r="BJ13" s="59"/>
       <c r="BK13" s="59"/>
     </row>
-    <row r="14" spans="1:92" s="1" customFormat="1">
-      <c r="A14" s="152"/>
+    <row r="14" spans="1:92" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="142"/>
       <c r="B14" s="112" t="s">
         <v>240</v>
       </c>
-      <c r="C14" s="141" t="s">
+      <c r="C14" s="148" t="s">
         <v>308</v>
       </c>
-      <c r="D14" s="142"/>
+      <c r="D14" s="149"/>
       <c r="E14" s="69" t="s">
         <v>241</v>
       </c>
@@ -4008,15 +4149,15 @@
       <c r="BJ14" s="59"/>
       <c r="BK14" s="59"/>
     </row>
-    <row r="15" spans="1:92" s="1" customFormat="1">
-      <c r="A15" s="152"/>
+    <row r="15" spans="1:92" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="142"/>
       <c r="B15" s="132" t="s">
         <v>309</v>
       </c>
-      <c r="C15" s="141" t="s">
+      <c r="C15" s="148" t="s">
         <v>308</v>
       </c>
-      <c r="D15" s="142"/>
+      <c r="D15" s="149"/>
       <c r="E15" s="69" t="s">
         <v>310</v>
       </c>
@@ -4143,15 +4284,15 @@
       <c r="BJ15" s="59"/>
       <c r="BK15" s="59"/>
     </row>
-    <row r="16" spans="1:92" s="1" customFormat="1">
-      <c r="A16" s="152"/>
+    <row r="16" spans="1:92" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="142"/>
       <c r="B16" s="112" t="s">
         <v>139</v>
       </c>
-      <c r="C16" s="143" t="s">
+      <c r="C16" s="150" t="s">
         <v>231</v>
       </c>
-      <c r="D16" s="144"/>
+      <c r="D16" s="151"/>
       <c r="E16" s="129" t="s">
         <v>307</v>
       </c>
@@ -4220,15 +4361,15 @@
       <c r="BJ16" s="50"/>
       <c r="BK16" s="50"/>
     </row>
-    <row r="17" spans="1:63" s="32" customFormat="1" ht="60">
-      <c r="A17" s="153"/>
+    <row r="17" spans="1:63" s="32" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="143"/>
       <c r="B17" s="112" t="s">
         <v>131</v>
       </c>
-      <c r="C17" s="141" t="s">
+      <c r="C17" s="148" t="s">
         <v>308</v>
       </c>
-      <c r="D17" s="142"/>
+      <c r="D17" s="149"/>
       <c r="E17" s="130" t="s">
         <v>301</v>
       </c>
@@ -4323,7 +4464,7 @@
       <c r="BJ17" s="53"/>
       <c r="BK17" s="53"/>
     </row>
-    <row r="18" spans="1:63" s="1" customFormat="1">
+    <row r="18" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="135"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -4378,7 +4519,7 @@
       <c r="BJ18" s="8"/>
       <c r="BK18" s="8"/>
     </row>
-    <row r="19" spans="1:63" s="1" customFormat="1">
+    <row r="19" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="9"/>
       <c r="C19" s="7"/>
       <c r="D19" s="9"/>
@@ -4435,29 +4576,29 @@
       <c r="BJ19" s="9"/>
       <c r="BK19" s="9"/>
     </row>
-    <row r="20" spans="1:63" s="1" customFormat="1">
+    <row r="20" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C20" s="26"/>
       <c r="AN20" s="23"/>
       <c r="AZ20" s="23"/>
     </row>
-    <row r="21" spans="1:63" s="1" customFormat="1">
+    <row r="21" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C21" s="26"/>
       <c r="AM21" s="43"/>
     </row>
-    <row r="22" spans="1:63" s="1" customFormat="1">
+    <row r="22" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C22" s="26"/>
       <c r="AM22" s="44"/>
       <c r="AZ22" s="26"/>
     </row>
-    <row r="23" spans="1:63" s="1" customFormat="1">
+    <row r="23" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C23" s="26"/>
       <c r="AM23" s="45"/>
     </row>
-    <row r="24" spans="1:63" s="1" customFormat="1">
+    <row r="24" spans="1:63" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C24" s="26"/>
       <c r="AM24" s="43"/>
     </row>
-    <row r="25" spans="1:63">
+    <row r="25" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C25" s="26"/>
       <c r="AM25" s="43"/>
       <c r="AS25" s="1"/>
@@ -4467,61 +4608,55 @@
       <c r="AW25" s="1"/>
       <c r="AX25" s="1"/>
     </row>
-    <row r="26" spans="1:63">
+    <row r="26" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C26" s="26"/>
       <c r="AM26" s="43"/>
     </row>
-    <row r="27" spans="1:63">
+    <row r="27" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C27" s="26"/>
       <c r="AM27" s="43"/>
     </row>
-    <row r="28" spans="1:63">
+    <row r="28" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C28" s="26"/>
     </row>
-    <row r="29" spans="1:63">
+    <row r="29" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C29" s="26"/>
     </row>
-    <row r="30" spans="1:63">
+    <row r="30" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C30" s="26"/>
     </row>
-    <row r="31" spans="1:63">
+    <row r="31" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C31" s="26"/>
     </row>
-    <row r="32" spans="1:63">
+    <row r="32" spans="1:63" x14ac:dyDescent="0.2">
       <c r="C32" s="26"/>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C33" s="26"/>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C34" s="26"/>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C35" s="26"/>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C36" s="26"/>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C37" s="26"/>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C38" s="26"/>
     </row>
-    <row r="41" spans="2:3" s="23" customFormat="1"/>
-    <row r="42" spans="2:3" s="23" customFormat="1">
+    <row r="41" spans="2:3" s="23" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="2:3" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B42" s="24"/>
     </row>
-    <row r="43" spans="2:3" s="23" customFormat="1"/>
-    <row r="44" spans="2:3" s="23" customFormat="1"/>
+    <row r="43" spans="2:3" s="23" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:3" s="23" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A8:A17"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C16:D16"/>
@@ -4533,6 +4668,12 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A8:A17"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157500000008" bottom="0.78740157500000008" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4549,17 +4690,17 @@
       <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="121.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="121.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>141</v>
       </c>
@@ -4578,7 +4719,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -4594,7 +4735,7 @@
       </c>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -4610,7 +4751,7 @@
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -4627,7 +4768,7 @@
         <v>3.6757114</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -4644,7 +4785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -4661,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -4678,7 +4819,7 @@
         <v>11.0395346</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -4695,7 +4836,7 @@
         <v>-9999.9003905999998</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -4712,7 +4853,7 @@
         <v>7.1244888</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -4730,7 +4871,7 @@
       </c>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -4747,7 +4888,7 @@
         <v>11.0395346</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -4764,7 +4905,7 @@
         <v>7.1244888</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -4781,7 +4922,7 @@
         <v>1018.2412109000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -4798,7 +4939,7 @@
         <v>0.27386700000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -4815,7 +4956,7 @@
         <v>0.1290026</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -4833,7 +4974,7 @@
       </c>
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -4850,7 +4991,7 @@
         <v>6.2584100000000004E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -4867,7 +5008,7 @@
         <v>-9999.9003905999998</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -4885,7 +5026,7 @@
       </c>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -4903,7 +5044,7 @@
       </c>
       <c r="F20" s="16"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -4920,7 +5061,7 @@
         <v>7.3349999999999999E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -4937,7 +5078,7 @@
         <v>-1.1363E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -4954,7 +5095,7 @@
         <v>-3.20965E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="14">
         <v>23</v>
       </c>
@@ -4971,7 +5112,7 @@
         <v>7.1272100000000005E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="14">
         <v>24</v>
       </c>
@@ -4988,7 +5129,7 @@
         <v>1.26479E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="14">
         <v>25</v>
       </c>
@@ -5005,7 +5146,7 @@
         <v>-1.6861999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="14">
         <v>26</v>
       </c>
@@ -5022,7 +5163,7 @@
         <v>-9999.9003905999998</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="14">
         <v>27</v>
       </c>
@@ -5039,7 +5180,7 @@
         <v>-9999.9003905999998</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="14">
         <v>28</v>
       </c>
@@ -5056,7 +5197,7 @@
         <v>-9999.9003905999998</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="14">
         <v>29</v>
       </c>
@@ -5073,7 +5214,7 @@
         <v>-9.4958999999999998E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="14">
         <v>30</v>
       </c>
@@ -5090,7 +5231,7 @@
         <v>6.4459999999999995E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="14">
         <v>31</v>
       </c>
@@ -5107,7 +5248,7 @@
         <v>3.6449999999999998E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="14">
         <v>32</v>
       </c>
@@ -5124,7 +5265,7 @@
         <v>-1.25138E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="14">
         <v>33</v>
       </c>
@@ -5141,7 +5282,7 @@
         <v>-1.9536000000000002E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="14">
         <v>34</v>
       </c>
@@ -5158,7 +5299,7 @@
         <v>2.3820999999999998E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -5173,7 +5314,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -5191,7 +5332,7 @@
       </c>
       <c r="F37" s="16"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -5208,7 +5349,7 @@
         <v>0.17921119999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -5225,7 +5366,7 @@
         <v>-21.172895400000002</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="14">
         <v>39</v>
       </c>
@@ -5242,7 +5383,7 @@
         <v>-9999.9003905999998</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -5259,7 +5400,7 @@
         <v>9.0208501999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="14">
         <v>41</v>
       </c>
@@ -5274,7 +5415,7 @@
         <v>0.30756699999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -5289,7 +5430,7 @@
         <v>0.29620600000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -5305,7 +5446,7 @@
       </c>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -5321,7 +5462,7 @@
       </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="14">
         <v>45</v>
       </c>
@@ -5336,7 +5477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -5351,7 +5492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -5366,7 +5507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -5381,7 +5522,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="14">
         <v>49</v>
       </c>
@@ -5398,7 +5539,7 @@
         <v>-9999.9003905999998</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -5415,7 +5556,7 @@
         <v>2.3820999999999998E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -5432,7 +5573,7 @@
         <v>27.4390869</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -5449,7 +5590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -5466,7 +5607,7 @@
         <v>160.20188899999999</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -5483,7 +5624,7 @@
         <v>6.5334162999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -5500,7 +5641,7 @@
         <v>11.630012499999999</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -5517,7 +5658,7 @@
         <v>9.4812908</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -5534,7 +5675,7 @@
         <v>11.0917139</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="14">
         <v>58</v>
       </c>
@@ -5551,7 +5692,7 @@
         <v>0.37518750000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="14">
         <v>59</v>
       </c>
@@ -5569,7 +5710,7 @@
       </c>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="14">
         <v>60</v>
       </c>
@@ -5586,7 +5727,7 @@
         <v>0.54817660000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="14">
         <v>61</v>
       </c>

</xml_diff>